<commit_message>
More working on adding reclamation data for the parsed rows
</commit_message>
<xml_diff>
--- a/monthly/src/reclamation/reclamation.xlsx
+++ b/monthly/src/reclamation/reclamation.xlsx
@@ -8,15 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roysegall/Sites/localhost/open_pension/monthly/src/reclamation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5827C6F9-5A7F-AF40-AE92-CCFEF328647D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAACD89-6BF7-4947-868E-D5F8D51648B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35820" yWindow="500" windowWidth="35840" windowHeight="20820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgrUUnK9+4pYG1alOzQcWxbR73wWQ=="/>
     </ext>
@@ -4182,8 +4190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C142" zoomScale="235" workbookViewId="0">
-      <selection activeCell="F155" sqref="F155"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="235" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>